<commit_message>
main branch permissions test
</commit_message>
<xml_diff>
--- a/practice_data.xlsx
+++ b/practice_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Personal data\Code and Research\visualization and storytelling from data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Personal data\Code and Research\visualization and storytelling from data\Effective_data_visualizations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A78878-9160-41B2-98A9-52B1C0D5D732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22F687A-F645-4AD5-84EA-D05B9CD126EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3C33E300-94BD-3244-BE01-92DFA5BF64CB}"/>
   </bookViews>
@@ -183,7 +183,7 @@
     <t>3. Clearer category labels that do not overlap to avoid confusion about where overlapping categories are placed.</t>
   </si>
   <si>
-    <t>Transformed Visual</t>
+    <t>Transformed Visuals - 2 trials</t>
   </si>
 </sst>
 </file>
@@ -366,7 +366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -422,7 +422,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10182,8 +10181,8 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10370,6 +10369,10 @@
       <c r="B26" s="14" t="s">
         <v>48</v>
       </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="12" t="s">
@@ -10569,7 +10572,7 @@
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C39" s="27">

</xml_diff>

<commit_message>
added a transformed stacked bar chart
</commit_message>
<xml_diff>
--- a/practice_data.xlsx
+++ b/practice_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Personal data\Code and Research\visualization and storytelling from data\Effective_data_visualizations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0502F601-4C5F-424E-ACED-D00BFC7BC76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01126772-4706-4F2F-B992-B2B7433F34BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3C33E300-94BD-3244-BE01-92DFA5BF64CB}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="110">
   <si>
     <t>Completion Rate</t>
   </si>
@@ -368,15 +368,6 @@
   </si>
   <si>
     <t>Survey item A</t>
-  </si>
-  <si>
-    <t>what I appreciate</t>
-  </si>
-  <si>
-    <t>The color choice to have the 2 agree and disagree groupd is very helpful for visual comparisons especially if the intent is to have the audience compare the groups as Disagree-Neutral-Agree</t>
-  </si>
-  <si>
-    <t>If there is any intention to have the audience compare the 2 groups of agree and disagree, the similar coloring takes from that, adding data labes would be very helpful</t>
   </si>
   <si>
     <t>agree</t>
@@ -3004,7 +2995,7 @@
           <c:x val="0.17429682281062944"/>
           <c:y val="0.14746888097136931"/>
           <c:w val="0.8040869076152416"/>
-          <c:h val="0.82029671264215975"/>
+          <c:h val="0.75141611191831315"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -15608,15 +15599,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16123,6 +16114,234 @@
             </a:rPr>
             <a:t>Strongly Agree</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>165905</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>31119</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65AFF00B-4558-BA27-B157-29DA0303767C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18297525" y="9229725"/>
+          <a:ext cx="6433355" cy="431169"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1700" b="1">
+              <a:solidFill>
+                <a:srgbClr val="515151"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Disagree </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1700" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1700" b="0">
+              <a:solidFill>
+                <a:srgbClr val="CBCBCB"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Neutral</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1700" b="1">
+              <a:solidFill>
+                <a:srgbClr val="CBCBCB"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1700" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>|</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1700" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1700" b="1">
+              <a:solidFill>
+                <a:srgbClr val="285E91"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Agree</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1700" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1700" b="1">
+            <a:solidFill>
+              <a:srgbClr val="285E91"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -16861,19 +17080,19 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.11676</cdr:x>
-      <cdr:y>0.06705</cdr:y>
+      <cdr:x>0.15878</cdr:x>
+      <cdr:y>0.02583</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.99222</cdr:x>
-      <cdr:y>0.15057</cdr:y>
+      <cdr:x>0.84964</cdr:x>
+      <cdr:y>0.17712</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 4">
+        <cdr:cNvPr id="5" name="TextBox 4">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32766390-F50E-1B99-8429-A68FA1103C13}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2317756-A293-5292-57D4-35E20F1194DE}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -16881,222 +17100,236 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="858034" y="311659"/>
-          <a:ext cx="6433355" cy="388211"/>
+          <a:off x="1166814" y="133351"/>
+          <a:ext cx="5076825" cy="781050"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
       </cdr:spPr>
-      <cdr:style>
-        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </cdr:style>
       <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:lvl1pPr marL="0" indent="0">
-            <a:defRPr sz="1100">
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
               <a:solidFill>
-                <a:schemeClr val="dk1"/>
+                <a:srgbClr val="515151"/>
               </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" indent="0">
-            <a:defRPr sz="1100">
+            </a:rPr>
+            <a:t>Survey Results</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:br>
+            <a:rPr kumimoji="0" lang="en-GB" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
               <a:solidFill>
-                <a:schemeClr val="dk1"/>
+                <a:srgbClr val="515151"/>
               </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" indent="0">
-            <a:defRPr sz="1100">
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-GB" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
               <a:solidFill>
-                <a:schemeClr val="dk1"/>
+                <a:srgbClr val="515151"/>
               </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-GB" sz="1700" b="1">
-              <a:solidFill>
-                <a:srgbClr val="515151"/>
-              </a:solidFill>
             </a:rPr>
             <a:t>Disagree </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-GB" sz="1700" b="1">
+            <a:rPr kumimoji="0" lang="en-GB" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
               <a:solidFill>
-                <a:schemeClr val="bg1">
+                <a:prstClr val="white">
                   <a:lumMod val="75000"/>
-                </a:schemeClr>
+                </a:prstClr>
               </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>| </a:t>
+            <a:t>|</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-GB" sz="1700" b="0">
+            <a:rPr kumimoji="0" lang="en-GB" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="50000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
               <a:solidFill>
                 <a:srgbClr val="CBCBCB"/>
               </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>Neutral</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-GB" sz="1700" b="1">
+            <a:rPr kumimoji="0" lang="en-GB" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
               <a:solidFill>
                 <a:srgbClr val="CBCBCB"/>
               </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-GB" sz="1700" b="1">
+            <a:rPr kumimoji="0" lang="en-GB" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
               <a:solidFill>
-                <a:schemeClr val="bg1">
+                <a:prstClr val="white">
                   <a:lumMod val="75000"/>
-                </a:schemeClr>
+                </a:prstClr>
               </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>|</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-GB" sz="1700" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1700" b="1">
+            <a:rPr kumimoji="0" lang="en-GB" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
               <a:solidFill>
                 <a:srgbClr val="285E91"/>
               </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>Agree</a:t>
           </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-GB" sz="1700" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
+            <a:rPr lang="en-US" sz="1100"/>
             <a:t> </a:t>
           </a:r>
-          <a:endParaRPr lang="en-GB" sz="1700" b="1">
-            <a:solidFill>
-              <a:srgbClr val="285E91"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.11515</cdr:x>
-      <cdr:y>0</cdr:y>
+      <cdr:x>0.18082</cdr:x>
+      <cdr:y>0.89668</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>1</cdr:x>
-      <cdr:y>0.07787</cdr:y>
+      <cdr:x>0.87557</cdr:x>
+      <cdr:y>1</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="4" name="TextBox 4">
+        <cdr:cNvPr id="6" name="TextBox 5">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DAED3F8-7F8C-954D-1BCE-0E2A5D43FD84}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28163045-26FA-3BD5-9896-F7AE61ED62AE}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -17104,147 +17337,26 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="846189" y="0"/>
-          <a:ext cx="6502350" cy="361959"/>
+          <a:off x="1328740" y="4629151"/>
+          <a:ext cx="5105400" cy="533400"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
       </cdr:spPr>
-      <cdr:style>
-        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </cdr:style>
       <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:lvl1pPr marL="0" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" indent="0">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-GB" sz="1700" b="1">
-              <a:solidFill>
-                <a:srgbClr val="515151"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Survey</a:t>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Some</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-GB" sz="1700" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="515151"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Results</a:t>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> follow up is neccesary to find out why such a large group of clients is nuetral on item C </a:t>
           </a:r>
-          <a:endParaRPr lang="en-GB" sz="1700" b="1">
-            <a:solidFill>
-              <a:srgbClr val="285E91"/>
-            </a:solidFill>
-          </a:endParaRPr>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -18584,8 +18696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F21ECAC-55FE-4F78-B585-C6E2752C0454}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18647,7 +18759,7 @@
         <v>101</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -18857,21 +18969,9 @@
       <c r="F13" s="35"/>
       <c r="G13" s="35"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I14" s="32" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I15" s="32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I16" s="32" t="s">
-        <v>111</v>
-      </c>
-    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>